<commit_message>
Featuers List updated with suggestion function
</commit_message>
<xml_diff>
--- a/featureslist/features list.xlsx
+++ b/featureslist/features list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Features List</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Order</t>
+  </si>
+  <si>
+    <t>Suggest journeys based on preferences</t>
   </si>
 </sst>
 </file>
@@ -428,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,29 +565,29 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -595,13 +598,24 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15">
         <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" s="5">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created a database uml diagram
</commit_message>
<xml_diff>
--- a/featureslist/features list.xlsx
+++ b/featureslist/features list.xlsx
@@ -2,16 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="8595" windowHeight="2595"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="8595" windowHeight="4095"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -93,7 +98,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,12 +108,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -125,7 +124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -136,10 +135,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,18 +437,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="74.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -463,7 +459,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -474,7 +470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -485,7 +481,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -496,7 +492,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -507,7 +503,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -518,7 +514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -529,7 +525,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -540,40 +536,41 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="7">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7">
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -584,7 +581,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -595,7 +592,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -606,7 +603,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -617,7 +614,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -630,7 +627,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -640,9 +642,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -652,8 +659,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>